<commit_message>
wrote parser for xl to pandas df
</commit_message>
<xml_diff>
--- a/data/becker menus.xlsx
+++ b/data/becker menus.xlsx
@@ -9,10 +9,10 @@
     <sheet state="visible" name="10292020" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="10302020" sheetId="5" r:id="rId8"/>
     <sheet state="visible" name="10312020" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="1112020" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="1122020" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="1132020" sheetId="9" r:id="rId12"/>
-    <sheet state="visible" name="1142020" sheetId="10" r:id="rId13"/>
+    <sheet state="visible" name="11012020" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="11022020" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="11032020" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="11042020" sheetId="10" r:id="rId13"/>
     <sheet state="visible" name="11252020" sheetId="11" r:id="rId14"/>
     <sheet state="visible" name="11272020" sheetId="12" r:id="rId15"/>
     <sheet state="visible" name="11282020" sheetId="13" r:id="rId16"/>
@@ -26,48 +26,47 @@
     <sheet state="visible" name="12082020" sheetId="21" r:id="rId24"/>
     <sheet state="visible" name="12092020" sheetId="22" r:id="rId25"/>
     <sheet state="visible" name="12102020" sheetId="23" r:id="rId26"/>
-    <sheet state="visible" name="4132021" sheetId="24" r:id="rId27"/>
-    <sheet state="visible" name="4142021" sheetId="25" r:id="rId28"/>
-    <sheet state="visible" name="4152021" sheetId="26" r:id="rId29"/>
-    <sheet state="visible" name="4162021" sheetId="27" r:id="rId30"/>
-    <sheet state="visible" name="4172021" sheetId="28" r:id="rId31"/>
-    <sheet state="visible" name="4182021" sheetId="29" r:id="rId32"/>
-    <sheet state="visible" name="4192021" sheetId="30" r:id="rId33"/>
-    <sheet state="visible" name="4202021" sheetId="31" r:id="rId34"/>
-    <sheet state="visible" name="4212021" sheetId="32" r:id="rId35"/>
-    <sheet state="visible" name="4222021" sheetId="33" r:id="rId36"/>
-    <sheet state="visible" name="542021" sheetId="34" r:id="rId37"/>
-    <sheet state="visible" name="552021" sheetId="35" r:id="rId38"/>
-    <sheet state="visible" name="562021" sheetId="36" r:id="rId39"/>
-    <sheet state="visible" name="572021" sheetId="37" r:id="rId40"/>
-    <sheet state="visible" name="582021" sheetId="38" r:id="rId41"/>
-    <sheet state="visible" name="592021" sheetId="39" r:id="rId42"/>
-    <sheet state="visible" name="5102021" sheetId="40" r:id="rId43"/>
-    <sheet state="visible" name="5112021" sheetId="41" r:id="rId44"/>
-    <sheet state="visible" name="5122021" sheetId="42" r:id="rId45"/>
-    <sheet state="visible" name="5242021" sheetId="43" r:id="rId46"/>
-    <sheet state="visible" name="5252021" sheetId="44" r:id="rId47"/>
-    <sheet state="visible" name="5262021" sheetId="45" r:id="rId48"/>
-    <sheet state="visible" name="5272021" sheetId="46" r:id="rId49"/>
-    <sheet state="visible" name="5282021" sheetId="47" r:id="rId50"/>
-    <sheet state="visible" name="5292021" sheetId="48" r:id="rId51"/>
-    <sheet state="visible" name="5302021" sheetId="49" r:id="rId52"/>
-    <sheet state="visible" name="9172021" sheetId="50" r:id="rId53"/>
-    <sheet state="visible" name="1072021" sheetId="51" r:id="rId54"/>
-    <sheet state="visible" name="1082021" sheetId="52" r:id="rId55"/>
-    <sheet state="visible" name="1092021" sheetId="53" r:id="rId56"/>
+    <sheet state="visible" name="04132021" sheetId="24" r:id="rId27"/>
+    <sheet state="visible" name="04142021" sheetId="25" r:id="rId28"/>
+    <sheet state="visible" name="04152021" sheetId="26" r:id="rId29"/>
+    <sheet state="visible" name="04162021" sheetId="27" r:id="rId30"/>
+    <sheet state="visible" name="04172021" sheetId="28" r:id="rId31"/>
+    <sheet state="visible" name="04182021" sheetId="29" r:id="rId32"/>
+    <sheet state="visible" name="04192021" sheetId="30" r:id="rId33"/>
+    <sheet state="visible" name="04202021" sheetId="31" r:id="rId34"/>
+    <sheet state="visible" name="04212021" sheetId="32" r:id="rId35"/>
+    <sheet state="visible" name="04222021" sheetId="33" r:id="rId36"/>
+    <sheet state="visible" name="05042021" sheetId="34" r:id="rId37"/>
+    <sheet state="visible" name="05052021" sheetId="35" r:id="rId38"/>
+    <sheet state="visible" name="05062021" sheetId="36" r:id="rId39"/>
+    <sheet state="visible" name="05072021" sheetId="37" r:id="rId40"/>
+    <sheet state="visible" name="05082021" sheetId="38" r:id="rId41"/>
+    <sheet state="visible" name="05092021" sheetId="39" r:id="rId42"/>
+    <sheet state="visible" name="05102021" sheetId="40" r:id="rId43"/>
+    <sheet state="visible" name="05112021" sheetId="41" r:id="rId44"/>
+    <sheet state="visible" name="05122021" sheetId="42" r:id="rId45"/>
+    <sheet state="visible" name="05242021" sheetId="43" r:id="rId46"/>
+    <sheet state="visible" name="05252021" sheetId="44" r:id="rId47"/>
+    <sheet state="visible" name="05262021" sheetId="45" r:id="rId48"/>
+    <sheet state="visible" name="05272021" sheetId="46" r:id="rId49"/>
+    <sheet state="visible" name="05282021" sheetId="47" r:id="rId50"/>
+    <sheet state="visible" name="05292021" sheetId="48" r:id="rId51"/>
+    <sheet state="visible" name="05302021" sheetId="49" r:id="rId52"/>
+    <sheet state="visible" name="09172021" sheetId="50" r:id="rId53"/>
+    <sheet state="visible" name="10072021" sheetId="51" r:id="rId54"/>
+    <sheet state="visible" name="10082021" sheetId="52" r:id="rId55"/>
+    <sheet state="visible" name="10092021" sheetId="53" r:id="rId56"/>
     <sheet state="visible" name="10102021" sheetId="54" r:id="rId57"/>
     <sheet state="visible" name="10112021" sheetId="55" r:id="rId58"/>
     <sheet state="visible" name="10122021" sheetId="56" r:id="rId59"/>
     <sheet state="visible" name="10132021" sheetId="57" r:id="rId60"/>
-    <sheet state="visible" name="10142021" sheetId="58" r:id="rId61"/>
-    <sheet state="visible" name="1242021" sheetId="59" r:id="rId62"/>
-    <sheet state="visible" name="1252021" sheetId="60" r:id="rId63"/>
-    <sheet state="visible" name="1262021" sheetId="61" r:id="rId64"/>
-    <sheet state="visible" name="1272021" sheetId="62" r:id="rId65"/>
-    <sheet state="visible" name="1282021" sheetId="63" r:id="rId66"/>
-    <sheet state="visible" name="1292021" sheetId="64" r:id="rId67"/>
-    <sheet state="visible" name="12102021" sheetId="65" r:id="rId68"/>
+    <sheet state="visible" name="12042021" sheetId="58" r:id="rId61"/>
+    <sheet state="visible" name="12052021" sheetId="59" r:id="rId62"/>
+    <sheet state="visible" name="12062021" sheetId="60" r:id="rId63"/>
+    <sheet state="visible" name="12072021" sheetId="61" r:id="rId64"/>
+    <sheet state="visible" name="12082021" sheetId="62" r:id="rId65"/>
+    <sheet state="visible" name="12092021" sheetId="63" r:id="rId66"/>
+    <sheet state="visible" name="12102021" sheetId="64" r:id="rId67"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -2283,10 +2282,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
-<file path=xl/drawings/drawing65.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
@@ -38988,7 +38983,158 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -39005,7 +39151,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2">
@@ -39015,7 +39161,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>510</v>
+        <v>520</v>
       </c>
     </row>
     <row r="4">
@@ -39025,7 +39171,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>511</v>
+        <v>521</v>
       </c>
     </row>
     <row r="6">
@@ -39035,7 +39181,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>512</v>
+        <v>522</v>
       </c>
     </row>
     <row r="8">
@@ -39045,7 +39191,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>513</v>
+        <v>523</v>
       </c>
     </row>
     <row r="10">
@@ -39055,101 +39201,91 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>514</v>
+        <v>524</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>443</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>60</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>525</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>515</v>
+        <v>526</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>516</v>
+        <v>527</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>517</v>
+        <v>528</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>518</v>
+        <v>529</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>519</v>
+        <v>443</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -39305,7 +39441,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
@@ -39315,17 +39451,17 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>520</v>
+        <v>530</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>521</v>
+        <v>432</v>
       </c>
     </row>
     <row r="6">
@@ -39335,7 +39471,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>522</v>
+        <v>531</v>
       </c>
     </row>
     <row r="8">
@@ -39345,32 +39481,32 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>523</v>
+        <v>532</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>436</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>524</v>
+        <v>533</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15">
@@ -39380,7 +39516,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>525</v>
+        <v>484</v>
       </c>
     </row>
     <row r="17">
@@ -39390,7 +39526,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>526</v>
+        <v>534</v>
       </c>
     </row>
     <row r="19">
@@ -39400,7 +39536,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>527</v>
+        <v>535</v>
       </c>
     </row>
     <row r="21">
@@ -39410,7 +39546,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>528</v>
+        <v>536</v>
       </c>
     </row>
     <row r="23">
@@ -39420,7 +39556,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>529</v>
+        <v>537</v>
       </c>
     </row>
     <row r="25">
@@ -39430,7 +39566,7 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>443</v>
+        <v>500</v>
       </c>
     </row>
     <row r="27">
@@ -39440,6 +39576,81 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -39490,7 +39701,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>531</v>
+        <v>543</v>
       </c>
     </row>
     <row r="8">
@@ -39500,176 +39711,186 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>532</v>
+        <v>544</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>436</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>533</v>
+        <v>545</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>436</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>8</v>
+        <v>546</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>484</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>534</v>
+        <v>459</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>535</v>
+        <v>547</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>536</v>
+        <v>527</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>537</v>
+        <v>548</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>500</v>
+        <v>549</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>15</v>
+        <v>499</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>8</v>
+        <v>443</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>538</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>539</v>
+        <v>550</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>540</v>
+        <v>551</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>541</v>
+        <v>552</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>542</v>
+        <v>553</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>443</v>
+        <v>554</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -39700,7 +39921,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>530</v>
+        <v>555</v>
       </c>
     </row>
     <row r="4">
@@ -39720,7 +39941,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>543</v>
+        <v>556</v>
       </c>
     </row>
     <row r="8">
@@ -39730,7 +39951,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>544</v>
+        <v>557</v>
       </c>
     </row>
     <row r="10">
@@ -39740,7 +39961,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>545</v>
+        <v>558</v>
       </c>
     </row>
     <row r="12">
@@ -39755,7 +39976,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15">
@@ -39775,7 +39996,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>459</v>
+        <v>559</v>
       </c>
     </row>
     <row r="19">
@@ -39795,7 +40016,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>527</v>
+        <v>560</v>
       </c>
     </row>
     <row r="23">
@@ -39805,7 +40026,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>548</v>
+        <v>561</v>
       </c>
     </row>
     <row r="25">
@@ -39815,12 +40036,12 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>549</v>
+        <v>562</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>499</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28">
@@ -39850,7 +40071,7 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>550</v>
+        <v>563</v>
       </c>
     </row>
     <row r="34">
@@ -39860,7 +40081,7 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>551</v>
+        <v>564</v>
       </c>
     </row>
     <row r="36">
@@ -39870,7 +40091,7 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>552</v>
+        <v>565</v>
       </c>
     </row>
     <row r="38">
@@ -39880,7 +40101,7 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>553</v>
+        <v>566</v>
       </c>
     </row>
     <row r="40">
@@ -39890,26 +40111,16 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>554</v>
+        <v>567</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -39940,7 +40151,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>555</v>
+        <v>530</v>
       </c>
     </row>
     <row r="4">
@@ -39960,7 +40171,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>556</v>
+        <v>568</v>
       </c>
     </row>
     <row r="8">
@@ -39970,7 +40181,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>557</v>
+        <v>569</v>
       </c>
     </row>
     <row r="10">
@@ -39980,7 +40191,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>558</v>
+        <v>570</v>
       </c>
     </row>
     <row r="12">
@@ -39990,7 +40201,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>546</v>
+        <v>571</v>
       </c>
     </row>
     <row r="14">
@@ -40015,7 +40226,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>559</v>
+        <v>450</v>
       </c>
     </row>
     <row r="19">
@@ -40025,7 +40236,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
     </row>
     <row r="21">
@@ -40035,7 +40246,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>560</v>
+        <v>573</v>
       </c>
     </row>
     <row r="23">
@@ -40045,7 +40256,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>561</v>
+        <v>574</v>
       </c>
     </row>
     <row r="25">
@@ -40055,7 +40266,7 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>562</v>
+        <v>575</v>
       </c>
     </row>
     <row r="27">
@@ -40090,7 +40301,7 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>563</v>
+        <v>550</v>
       </c>
     </row>
     <row r="34">
@@ -40100,7 +40311,7 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>564</v>
+        <v>551</v>
       </c>
     </row>
     <row r="36">
@@ -40110,7 +40321,7 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>565</v>
+        <v>576</v>
       </c>
     </row>
     <row r="38">
@@ -40120,7 +40331,7 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>566</v>
+        <v>577</v>
       </c>
     </row>
     <row r="40">
@@ -40130,16 +40341,26 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>567</v>
+        <v>578</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -40170,246 +40391,6 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="1" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="1" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
         <v>431</v>
       </c>
     </row>

</xml_diff>